<commit_message>
Adiciona arquivo com resumo das métricas de avaliação
</commit_message>
<xml_diff>
--- a/resultados_cotton.xlsx
+++ b/resultados_cotton.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenau\Desktop\Andressa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenau\Documents\GitHub\cotton_candy_spectral_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DEC772-11B3-4A58-B4BE-11D0F6BD4841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246FCE7E-30D6-4A8E-9ACE-05302377F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D296E6EB-D2C7-4C7B-AC46-64E9FC4237DE}"/>
   </bookViews>
@@ -96,9 +96,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -290,18 +298,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,7 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,71 +345,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -744,30 +700,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14"/>
-      <c r="O1" s="16" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="O1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="18"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -829,7 +785,7 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
@@ -838,49 +794,49 @@
       <c r="D3">
         <v>2.5201065220254368</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>1.127220969087652</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.81993359409013122</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
         <v>0.83573350000000002</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3">
         <v>2.3106205000000002</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>1.0197835</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>0.83573339999999996</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="22">
+      <c r="P3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="11">
         <f>C3-J3</f>
         <v>-1.5799905909869461E-2</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="11">
         <f t="shared" ref="R3:T12" si="0">D3-K3</f>
         <v>0.20948602202543665</v>
       </c>
-      <c r="S3" s="22">
+      <c r="S3" s="11">
         <f t="shared" si="0"/>
         <v>0.10743746908765206</v>
       </c>
-      <c r="T3" s="23">
+      <c r="T3" s="12">
         <f t="shared" si="0"/>
         <v>-1.5799805909868736E-2</v>
       </c>
@@ -889,58 +845,58 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
         <v>0.79404172537923268</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>2.8884464746932781</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>1.3683505637388109</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.73465596509312792</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4">
         <v>0.81014649999999999</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>2.6785328000000002</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>1.2069063</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>0.77254120000000004</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="24">
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="13">
         <f t="shared" ref="Q4:Q12" si="1">C4-J4</f>
         <v>-1.6104774620767315E-2</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="13">
         <f t="shared" si="0"/>
         <v>0.20991367469327793</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="13">
         <f t="shared" si="0"/>
         <v>0.16144426373881093</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="14">
         <f t="shared" si="0"/>
         <v>-3.7885234906872123E-2</v>
       </c>
@@ -949,58 +905,58 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
         <v>0.61941596942462884</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>1.2500358601054189</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>0.19026926159777099</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.6194159694246284</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
         <v>0.59908530000000004</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>1.3204777000000001</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>0.1906601</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>0.59908519999999998</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="24">
+      <c r="P5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="13">
         <f t="shared" si="1"/>
         <v>2.03306694246288E-2</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="13">
         <f t="shared" si="0"/>
         <v>-7.0441839894581193E-2</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="13">
         <f t="shared" si="0"/>
         <v>-3.9083840222900457E-4</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="14">
         <f t="shared" si="0"/>
         <v>2.0330769424628414E-2</v>
       </c>
@@ -1009,58 +965,58 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
         <v>0.50072627297001404</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>1.6384814216378061</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>0.23450531881980849</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.42187907286094373</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6">
         <v>0.48299999999999998</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6">
         <v>1.7044386</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6">
         <v>0.23986730000000001</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.37266899999999997</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="24">
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="13">
         <f t="shared" si="1"/>
         <v>1.7726272970014056E-2</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="13">
         <f t="shared" si="0"/>
         <v>-6.5957178362193947E-2</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="13">
         <f t="shared" si="0"/>
         <v>-5.3619811801915163E-3</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="14">
         <f t="shared" si="0"/>
         <v>4.9210072860943754E-2</v>
       </c>
@@ -1069,58 +1025,58 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
         <v>0.64140712202254158</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>0.40261988698445023</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>0.35116475002874192</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.64140712202254024</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
         <v>0.65833660000000005</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7">
         <v>0.3784342</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7">
         <v>0.3285785</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>0.65833660000000005</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="24">
+      <c r="P7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="13">
         <f t="shared" si="1"/>
         <v>-1.6929477977458474E-2</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="13">
         <f t="shared" si="0"/>
         <v>2.4185686984450228E-2</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="13">
         <f t="shared" si="0"/>
         <v>2.2586250028741928E-2</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="14">
         <f t="shared" si="0"/>
         <v>-1.6929477977459806E-2</v>
       </c>
@@ -1129,58 +1085,58 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
         <v>0.53329484265160709</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>0.5280357467405109</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>0.4459264415167446</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.42176246456205629</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8">
         <v>0.5164569</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8">
         <v>0.53616830000000004</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8">
         <v>0.45295530000000001</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>0.35812100000000002</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="24">
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="13">
         <f t="shared" si="1"/>
         <v>1.6837942651607096E-2</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="13">
         <f t="shared" si="0"/>
         <v>-8.1325532594891392E-3</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="13">
         <f t="shared" si="0"/>
         <v>-7.0288584832554069E-3</v>
       </c>
-      <c r="T8" s="25">
+      <c r="T8" s="14">
         <f t="shared" si="0"/>
         <v>6.3641464562056271E-2</v>
       </c>
@@ -1189,58 +1145,58 @@
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
         <v>0.64968274785335189</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>179.71628555275771</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>60.827106833452874</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.64968274785335345</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
         <v>0.64941970000000004</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9">
         <v>178.34014999999999</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9">
         <v>57.329231</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>0.64941970000000004</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="24">
+      <c r="P9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="13">
         <f t="shared" si="1"/>
         <v>2.6304785335184988E-4</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="13">
         <f t="shared" si="0"/>
         <v>1.3761355527577166</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="13">
         <f t="shared" si="0"/>
         <v>3.4978758334528735</v>
       </c>
-      <c r="T9" s="25">
+      <c r="T9" s="14">
         <f t="shared" si="0"/>
         <v>2.6304785335340419E-4</v>
       </c>
@@ -1249,58 +1205,58 @@
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
         <v>0.52081720504666384</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>245.1575041810685</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>80.642385265642574</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>0.38426486625308098</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10">
         <v>0.5135651</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10">
         <v>247.25973999999999</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10">
         <v>78.954025000000001</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>0.34263549999999998</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="24">
+      <c r="P10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="13">
         <f t="shared" si="1"/>
         <v>7.2521050466638481E-3</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="13">
         <f t="shared" si="0"/>
         <v>-2.10223581893149</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="13">
         <f t="shared" si="0"/>
         <v>1.6883602656425722</v>
       </c>
-      <c r="T10" s="25">
+      <c r="T10" s="14">
         <f t="shared" si="0"/>
         <v>4.1629366253081002E-2</v>
       </c>
@@ -1309,118 +1265,118 @@
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
         <v>0.64744304045116219</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>5.4078838621350762</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>1.910040297746731</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.64744304045116263</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="15">
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11">
         <v>0.62050680000000003</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11">
         <v>5.8451237999999996</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11">
         <v>1.9071712000000001</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>0.62050689999999997</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="24">
+      <c r="P11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="13">
         <f t="shared" si="1"/>
         <v>2.6936240451162163E-2</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="13">
         <f t="shared" si="0"/>
         <v>-0.43723993786492343</v>
       </c>
-      <c r="S11" s="24">
+      <c r="S11" s="13">
         <f t="shared" si="0"/>
         <v>2.869097746730942E-3</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11" s="14">
         <f t="shared" si="0"/>
         <v>2.693614045116266E-2</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
         <v>0.62062587246848666</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>5.8131192037186654</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>2.0393230328797181</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>0.5981015966807981</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="7">
+      <c r="I12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="6">
         <v>0.59692199999999995</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>6.2089261999999996</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>2.0061643</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>0.58487420000000001</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="26">
+      <c r="P12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="15">
         <f t="shared" si="1"/>
         <v>2.3703872468486709E-2</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="15">
         <f t="shared" si="0"/>
         <v>-0.3958069962813342</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="15">
         <f t="shared" si="0"/>
         <v>3.3158732879718045E-2</v>
       </c>
-      <c r="T12" s="27">
+      <c r="T12" s="16">
         <f t="shared" si="0"/>
         <v>1.3227396680798087E-2</v>
       </c>
@@ -1465,30 +1421,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14"/>
-      <c r="O1" s="16" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="O1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="18"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1550,58 +1506,58 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>0.80517434260485121</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>2.711639164099223</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>1.1488379291648441</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.80517434260485143</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
         <v>0.8177816</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3">
         <v>2.5650100999999998</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>1.0630331</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>0.81778169999999994</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="22">
+      <c r="P3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="11">
         <f>C3-J3</f>
         <v>-1.2607257395148785E-2</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="11">
         <f t="shared" ref="R3:T12" si="0">D3-K3</f>
         <v>0.14662906409922316</v>
       </c>
-      <c r="S3" s="22">
+      <c r="S3" s="11">
         <f t="shared" si="0"/>
         <v>8.580482916484411E-2</v>
       </c>
-      <c r="T3" s="23">
+      <c r="T3" s="12">
         <f t="shared" si="0"/>
         <v>-1.2607357395148511E-2</v>
       </c>
@@ -1610,58 +1566,58 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
         <v>0.77939886678517356</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>3.0676033397474058</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>1.331391679010095</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.73833821718791581</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4">
         <v>0.78984840000000001</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>2.9583436999999999</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>1.2371198000000001</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>0.75602550000000002</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="24">
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="13">
         <f t="shared" ref="Q4:Q12" si="1">C4-J4</f>
         <v>-1.0449533214826445E-2</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="13">
         <f t="shared" si="0"/>
         <v>0.10925963974740593</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="13">
         <f t="shared" si="0"/>
         <v>9.4271879010094928E-2</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="14">
         <f t="shared" si="0"/>
         <v>-1.7687282812084204E-2</v>
       </c>
@@ -1670,58 +1626,58 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>0.6243669284832003</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>1.240089264609229</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>0.1919195916110745</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.62436692848319875</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
         <v>0.64774880000000001</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>1.1586405</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>0.18073919999999999</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>0.64774880000000001</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="24">
+      <c r="P5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="13">
         <f t="shared" si="1"/>
         <v>-2.3381871516799713E-2</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="13">
         <f t="shared" si="0"/>
         <v>8.1448764609229007E-2</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="13">
         <f t="shared" si="0"/>
         <v>1.1180391611074508E-2</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="14">
         <f t="shared" si="0"/>
         <v>-2.3381871516801267E-2</v>
       </c>
@@ -1730,58 +1686,58 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>0.51809218535763268</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>1.5921543247028549</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>0.24275387139029961</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.39902344592365668</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6">
         <v>0.52827610000000003</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6">
         <v>1.5530785</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6">
         <v>0.23593330000000001</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.40659859999999998</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="24">
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="13">
         <f t="shared" si="1"/>
         <v>-1.0183914642367342E-2</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="13">
         <f t="shared" si="0"/>
         <v>3.9075824702854867E-2</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="13">
         <f t="shared" si="0"/>
         <v>6.8205713902995957E-3</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="14">
         <f t="shared" si="0"/>
         <v>-7.5751540763432934E-3</v>
       </c>
@@ -1790,58 +1746,58 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>0.49466579089479201</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>0.5687060065510533</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>0.39750201142485758</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.49466579089479201</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
         <v>0.56413999999999997</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7">
         <v>0.47895789999999999</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7">
         <v>0.36707849999999997</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>0.56413970000000002</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="24">
+      <c r="P7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="13">
         <f t="shared" si="1"/>
         <v>-6.9474209105207962E-2</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="13">
         <f t="shared" si="0"/>
         <v>8.9748106551053308E-2</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="13">
         <f t="shared" si="0"/>
         <v>3.0423511424857608E-2</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="14">
         <f t="shared" si="0"/>
         <v>-6.9473909105208009E-2</v>
       </c>
@@ -1850,58 +1806,58 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
         <v>0.45327630229049742</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>0.61757413262141247</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>0.43480915647669183</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.39535926801741139</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8">
         <v>0.4944402</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8">
         <v>0.55658110000000005</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8">
         <v>0.42934149999999999</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>0.41053600000000001</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="24">
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="13">
         <f t="shared" si="1"/>
         <v>-4.1163897709502573E-2</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="13">
         <f t="shared" si="0"/>
         <v>6.0993032621412424E-2</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="13">
         <f t="shared" si="0"/>
         <v>5.4676564766918401E-3</v>
       </c>
-      <c r="T8" s="25">
+      <c r="T8" s="14">
         <f t="shared" si="0"/>
         <v>-1.517673198258862E-2</v>
       </c>
@@ -1910,58 +1866,58 @@
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
         <v>0.61270654828965221</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>199.11925757342621</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>62.911160338804287</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.61270654828965176</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
         <v>0.65845200000000004</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9">
         <v>173.04422</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9">
         <v>56.354464999999998</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>0.65845200000000004</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="24">
+      <c r="P9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="13">
         <f t="shared" si="1"/>
         <v>-4.5745451710347829E-2</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="13">
         <f t="shared" si="0"/>
         <v>26.075037573426215</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="13">
         <f t="shared" si="0"/>
         <v>6.556695338804289</v>
       </c>
-      <c r="T9" s="25">
+      <c r="T9" s="14">
         <f t="shared" si="0"/>
         <v>-4.5745451710348273E-2</v>
       </c>
@@ -1970,58 +1926,58 @@
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
         <v>0.4980083127535585</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>258.2357080583688</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>79.662443980436819</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>0.37899940626834511</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10">
         <v>0.55718529999999999</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10">
         <v>225.13936000000001</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10">
         <v>74.451271000000006</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>0.41066570000000002</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="24">
+      <c r="P10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="13">
         <f t="shared" si="1"/>
         <v>-5.9176987246441493E-2</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="13">
         <f t="shared" si="0"/>
         <v>33.09634805836879</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="13">
         <f t="shared" si="0"/>
         <v>5.2111729804368139</v>
       </c>
-      <c r="T10" s="25">
+      <c r="T10" s="14">
         <f t="shared" si="0"/>
         <v>-3.1666293731654915E-2</v>
       </c>
@@ -2030,118 +1986,118 @@
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
         <v>0.6726734889966427</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>5.0001820590740236</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>1.800229857848642</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.67267348899664148</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="15">
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11">
         <v>0.68146879999999999</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11">
         <v>4.9062123</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11">
         <v>1.7361149</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>0.68146879999999999</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="24">
+      <c r="P11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="13">
         <f t="shared" si="1"/>
         <v>-8.7953110033572868E-3</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="13">
         <f t="shared" si="0"/>
         <v>9.3969759074023607E-2</v>
       </c>
-      <c r="S11" s="24">
+      <c r="S11" s="13">
         <f t="shared" si="0"/>
         <v>6.4114957848641962E-2</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11" s="14">
         <f t="shared" si="0"/>
         <v>-8.795311003358508E-3</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
         <v>0.64270345990556199</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>5.4435342672436269</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>1.996812083006219</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>0.59728328797603902</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="7">
+      <c r="I12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="6">
         <v>0.64432339999999999</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>5.4757885999999996</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>1.9687713</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>0.59504389999999996</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="26">
+      <c r="P12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="15">
         <f t="shared" si="1"/>
         <v>-1.6199400944379994E-3</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="15">
         <f t="shared" si="0"/>
         <v>-3.2254332756372683E-2</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="15">
         <f t="shared" si="0"/>
         <v>2.8040783006219039E-2</v>
       </c>
-      <c r="T12" s="27">
+      <c r="T12" s="16">
         <f t="shared" si="0"/>
         <v>2.2393879760390645E-3</v>
       </c>
@@ -2166,7 +2122,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,30 +2141,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14"/>
-      <c r="O1" s="16" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="O1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="18"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2267,61 +2223,61 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="21">
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.84687522119745073</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="10">
         <v>2.1440969027301029</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="10">
         <v>1.0397824956310671</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="8">
         <v>0.84687522119744874</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
         <v>0.80306520000000003</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3">
         <v>2.7721672000000002</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>1.1051264999999999</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>0.80306520000000003</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="22">
+      <c r="P3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="11">
         <f>C3-J3</f>
         <v>4.3810021197450699E-2</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="11">
         <f t="shared" ref="R3:T12" si="0">D3-K3</f>
         <v>-0.62807029726989727</v>
       </c>
-      <c r="S3" s="22">
+      <c r="S3" s="11">
         <f t="shared" si="0"/>
         <v>-6.534400436893284E-2</v>
       </c>
-      <c r="T3" s="23">
+      <c r="T3" s="12">
         <f t="shared" si="0"/>
         <v>4.3810021197448701E-2</v>
       </c>
@@ -2330,58 +2286,58 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
         <v>0.80855150930013575</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>2.6811707095913828</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>1.2409121929124789</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.78190657434404054</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4">
         <v>0.78600979999999998</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>3.0183339</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>1.2179475</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>0.76352880000000001</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="24">
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="13">
         <f t="shared" ref="Q4:Q12" si="1">C4-J4</f>
         <v>2.254170930013577E-2</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="13">
         <f t="shared" si="0"/>
         <v>-0.3371631904086172</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="13">
         <f t="shared" si="0"/>
         <v>2.2964692912478935E-2</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="14">
         <f t="shared" si="0"/>
         <v>1.8377774344040532E-2</v>
       </c>
@@ -2390,58 +2346,58 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>0.73489838052279488</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>0.86993323661404354</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>0.1590784931502259</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.7348983805227961</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
         <v>0.61363380000000001</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>1.2708534</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>0.18928919999999999</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>0.61363369999999995</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="24">
+      <c r="P5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="13">
         <f t="shared" si="1"/>
         <v>0.12126458052279487</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="13">
         <f t="shared" si="0"/>
         <v>-0.40092016338595649</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="13">
         <f t="shared" si="0"/>
         <v>-3.0210706849774088E-2</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="14">
         <f t="shared" si="0"/>
         <v>0.12126468052279615</v>
       </c>
@@ -2450,58 +2406,58 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>0.54055335105592783</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>1.5087408190727869</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>0.23232408196760049</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.43457122901327561</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6">
         <v>0.54476480000000005</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6">
         <v>1.4960203000000001</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6">
         <v>0.22032009999999999</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.48253790000000002</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="24">
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="13">
         <f t="shared" si="1"/>
         <v>-4.2114489440722158E-3</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="13">
         <f t="shared" si="0"/>
         <v>1.2720519072786818E-2</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="13">
         <f t="shared" si="0"/>
         <v>1.2003981967600497E-2</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="14">
         <f t="shared" si="0"/>
         <v>-4.7966670986724413E-2</v>
       </c>
@@ -2510,58 +2466,58 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>0.6086435674804006</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>0.4390035190982437</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>0.36697974976150399</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.60864356748040049</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
         <v>0.52618500000000001</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7">
         <v>0.52066579999999996</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7">
         <v>0.3827275</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>0.52618500000000001</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="24">
+      <c r="P7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="13">
         <f t="shared" si="1"/>
         <v>8.2458567480400591E-2</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="13">
         <f t="shared" si="0"/>
         <v>-8.1662280901756257E-2</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="13">
         <f t="shared" si="0"/>
         <v>-1.5747750238496006E-2</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="14">
         <f t="shared" si="0"/>
         <v>8.245856748040048E-2</v>
       </c>
@@ -2570,58 +2526,58 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
         <v>0.55178277930605368</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>0.50240773883667722</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>0.41663893110056649</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.49556179361474068</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8">
         <v>0.49563420000000002</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8">
         <v>0.55263039999999997</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8">
         <v>0.40503250000000002</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>0.4753964</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="24">
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="13">
         <f t="shared" si="1"/>
         <v>5.6148579306053659E-2</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="13">
         <f t="shared" si="0"/>
         <v>-5.0222661163322746E-2</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="13">
         <f t="shared" si="0"/>
         <v>1.1606431100566472E-2</v>
       </c>
-      <c r="T8" s="25">
+      <c r="T8" s="14">
         <f t="shared" si="0"/>
         <v>2.0165393614740679E-2</v>
       </c>
@@ -2630,58 +2586,58 @@
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
         <v>0.66626683894107286</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>171.20742487079741</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>59.370814032732788</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.66626683894107308</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
         <v>0.56623840000000003</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9">
         <v>219.76398</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9">
         <v>63.507942</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>0.56623829999999997</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="24">
+      <c r="P9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="13">
         <f t="shared" si="1"/>
         <v>0.10002843894107283</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="13">
         <f t="shared" si="0"/>
         <v>-48.556555129202593</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="13">
         <f t="shared" si="0"/>
         <v>-4.1371279672672117</v>
       </c>
-      <c r="T9" s="25">
+      <c r="T9" s="14">
         <f t="shared" si="0"/>
         <v>0.10002853894107311</v>
       </c>
@@ -2690,58 +2646,58 @@
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
         <v>0.55747448063660132</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>227.08623974317419</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>73.834108540666449</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>0.48386010848931432</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10">
         <v>0.52548539999999999</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10">
         <v>239.85991999999999</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10">
         <v>70.728554000000003</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>0.46812809999999999</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="24">
+      <c r="P10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="13">
         <f t="shared" si="1"/>
         <v>3.198908063660133E-2</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="13">
         <f t="shared" si="0"/>
         <v>-12.773680256825799</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="13">
         <f t="shared" si="0"/>
         <v>3.1055545406664464</v>
       </c>
-      <c r="T10" s="25">
+      <c r="T10" s="14">
         <f t="shared" si="0"/>
         <v>1.5732008489314331E-2</v>
       </c>
@@ -2750,124 +2706,124 @@
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
         <v>0.76586803428254535</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>3.593486468355088</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>1.5563355442717171</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.76586803428254557</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="15">
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11">
         <v>0.65572680000000005</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11">
         <v>5.3027062000000003</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11">
         <v>1.8049040999999999</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>0.65572680000000005</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="24">
+      <c r="P11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="13">
         <f t="shared" si="1"/>
         <v>0.1101412342825453</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="13">
         <f t="shared" si="0"/>
         <v>-1.7092197316449123</v>
       </c>
-      <c r="S11" s="24">
+      <c r="S11" s="13">
         <f t="shared" si="0"/>
         <v>-0.24856855572828285</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11" s="14">
         <f t="shared" si="0"/>
         <v>0.11014123428254552</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
         <v>0.72712664602882837</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>4.1469199518980453</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>1.9224499757886651</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>0.64275650077831448</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="7">
+      <c r="I12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="6">
         <v>0.63514170000000003</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>5.6225437999999999</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>1.9006187000000001</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>0.62259529999999996</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="26">
+      <c r="P12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="15">
         <f t="shared" si="1"/>
         <v>9.198494602882834E-2</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="15">
         <f t="shared" si="0"/>
         <v>-1.4756238481019546</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="15">
         <f t="shared" si="0"/>
         <v>2.183127578866495E-2</v>
       </c>
-      <c r="T12" s="27">
+      <c r="T12" s="16">
         <f t="shared" si="0"/>
         <v>2.0161200778314514E-2</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="O14" t="s">
+      <c r="O14" s="26" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>